<commit_message>
Constraint for diminished chord done + progress on the doubling of notes for chords in fundamental state
</commit_message>
<xml_diff>
--- a/ContraintesDuha/AvancementImplementationRegles.xlsx
+++ b/ContraintesDuha/AvancementImplementationRegles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sprockeelsd/Documents/Doctorat/MusicalConstraints/MusicConstraints/ContraintesDuha/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA49E4A4-49F6-3541-B328-C16BA9A88AD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD66247C-F105-6848-9B23-04ADDD21FDFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3840" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{2DB875F2-6E32-A84C-97E1-7DDD4CAE854B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Ne jamais doubler la septième de la tonalité</t>
   </si>
@@ -57,13 +57,46 @@
   </si>
   <si>
     <t>Doubler de préférence la basse</t>
+  </si>
+  <si>
+    <t>Quand on enchaine 2 accords dont l'intervalle entre les basses est une quarte ou une quinte, on garde la note commune et on enchaine les autres au plus près</t>
+  </si>
+  <si>
+    <t>Quand on enchaine 2 accords dont l’intervalle entre les basses est une tierce (montante ou descendante), on garde les 2 notes communes et on enchaine les autres parties au plus près</t>
+  </si>
+  <si>
+    <t>Quand on enchaine 2 accords dont l’intervalle entre les basses est une seconde, toutes les voix vont par mouvement contraire à la basse pour éviter les quintes et octaves consécutives</t>
+  </si>
+  <si>
+    <t>Il est interdit de faire 2  quintes ou octaves consécutives même par mouvement contraire</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>L’accord de quinte diminuée du second degré du mode mineur et l’accord de septième degré du mode majeur seront de préférence utilisés à 3 voix, les doublures de notes dans ces accords étant d’un effet peu heureux</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -71,13 +104,32 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="1"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -92,10 +144,19 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -414,7 +475,7 @@
   <dimension ref="A2:C39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -432,7 +493,7 @@
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
@@ -451,12 +512,38 @@
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="6" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="8" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="9" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
     <row r="10" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added constraint for voice movement in successive fundamental state chords
Currently does not work properly
- Also kept working on tritone resolution which still doesn't work
- Cleaned up the FourVoiceTextureConstraint.h file
</commit_message>
<xml_diff>
--- a/ContraintesDuha/AvancementImplementationRegles.xlsx
+++ b/ContraintesDuha/AvancementImplementationRegles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sprockeelsd/Documents/Doctorat/MusicalConstraints/MusicConstraints/ContraintesDuha/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD66FD00-DCF4-9844-AF84-609F57A33E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B713DC0A-00EB-AF4A-AD3D-54444B8F272C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-3840" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{2DB875F2-6E32-A84C-97E1-7DDD4CAE854B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>Ne jamais doubler la septième de la tonalité</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> équivalent à minimiser le mouvement dans une même voix + le mouvement inverse par rapport à la basse pour les accords à une seconde d'intervalle</t>
+  </si>
+  <si>
+    <t>Minimiser le mouvement dans une même voix (attention aux intervalles négatifs -&gt; valeur absolue?)</t>
   </si>
 </sst>
 </file>
@@ -147,7 +153,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -160,6 +166,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -475,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{303EE715-FBAC-9E42-A5C1-E447E5CC7652}">
-  <dimension ref="A2:C39"/>
+  <dimension ref="A2:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,85 +514,99 @@
     </row>
     <row r="3" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="B5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="104" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B6" s="1" t="s">
+    <row r="7" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B7" s="3" t="s">
+    <row r="8" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
+    <row r="9" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="4" t="s">
+    <row r="10" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="11" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="12" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="13" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="14" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="15" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="17" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="18" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="19" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="20" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="22" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="23" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="24" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="25" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="26" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="27" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="28" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" s="1" customFormat="1" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="17" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="18" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="19" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="20" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="21" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="22" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="23" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="24" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="25" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="27" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="28" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="29" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="63" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A7:A9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added the constraint that parallel 1/5/8 are forbidden
- Made the distinction between generic/chord/interval csts in the problem consructor
- Added the constraint that a given interval can be forbidden to appear twice in a row between the same voices
</commit_message>
<xml_diff>
--- a/ContraintesDuha/AvancementImplementationRegles.xlsx
+++ b/ContraintesDuha/AvancementImplementationRegles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sprockeelsd/Documents/Doctorat/MusicalConstraints/MusicConstraints/ContraintesDuha/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B713DC0A-00EB-AF4A-AD3D-54444B8F272C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E19D2AB3-6129-D04D-A2E3-08D29492CF24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3840" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{2DB875F2-6E32-A84C-97E1-7DDD4CAE854B}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17740" xr2:uid="{2DB875F2-6E32-A84C-97E1-7DDD4CAE854B}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Ne jamais doubler la septième de la tonalité</t>
   </si>
@@ -92,13 +92,16 @@
     <t>Fait mais à modifier pour ajouter la notion de priorité</t>
   </si>
   <si>
-    <t xml:space="preserve"> </t>
-  </si>
-  <si>
     <t xml:space="preserve"> équivalent à minimiser le mouvement dans une même voix + le mouvement inverse par rapport à la basse pour les accords à une seconde d'intervalle</t>
   </si>
   <si>
     <t>Minimiser le mouvement dans une même voix (attention aux intervalles négatifs -&gt; valeur absolue?)</t>
+  </si>
+  <si>
+    <t>Fait</t>
+  </si>
+  <si>
+    <t>Fait dans la minimisation</t>
   </si>
 </sst>
 </file>
@@ -153,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -166,9 +169,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="4"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -490,7 +490,7 @@
   <dimension ref="A2:C40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -509,14 +509,13 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" s="5"/>
+        <v>13</v>
+      </c>
     </row>
     <row r="4" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
@@ -533,34 +532,40 @@
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>2</v>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="104" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>13</v>
+      <c r="A7" s="5" t="s">
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C7" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="6"/>
+      <c r="A8" s="5"/>
       <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
+      <c r="C8" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="6"/>
+      <c r="A9" s="5"/>
       <c r="B9" s="1" t="s">
         <v>9</v>
       </c>

</xml_diff>